<commit_message>
cambios hechos en una segunda rama de prueba
- Incluye nueva estrategia de lectura, no por color, si por si hay celda pintada
- Es capaz de agregar nuevos assets
- Esperamos que una nueva version sea leyendo desde la base de datos
</commit_message>
<xml_diff>
--- a/test_maestro_luis/Maestro Enero 2023.xlsx
+++ b/test_maestro_luis/Maestro Enero 2023.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10123" uniqueCount="1377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10134" uniqueCount="1378">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -4154,6 +4154,9 @@
   </si>
   <si>
     <t xml:space="preserve">Chassis cabina NQR 919 VL20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AABB11</t>
   </si>
 </sst>
 </file>
@@ -4202,7 +4205,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4225,6 +4228,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF481D32"/>
         <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -4287,7 +4296,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4333,6 +4342,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4461,15 +4478,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1937"/>
+  <dimension ref="A1:N1938"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A885" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L217" activeCellId="0" sqref="L217"/>
+      <selection pane="bottomLeft" activeCell="A937" activeCellId="0" sqref="937:937"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1010" style="0" width="9.14"/>
   </cols>
@@ -45404,21 +45421,49 @@
         <v>31</v>
       </c>
     </row>
-    <row r="937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A937" s="4"/>
-      <c r="B937" s="4"/>
-      <c r="C937" s="4"/>
-      <c r="D937" s="4"/>
-      <c r="E937" s="4"/>
-      <c r="F937" s="4"/>
-      <c r="G937" s="4"/>
-      <c r="H937" s="4"/>
-      <c r="I937" s="4"/>
-      <c r="J937" s="4"/>
-      <c r="K937" s="4"/>
-      <c r="L937" s="4"/>
-      <c r="M937" s="4"/>
-      <c r="N937" s="4"/>
+    <row r="937" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A937" s="12" t="n">
+        <v>936</v>
+      </c>
+      <c r="B937" s="12" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C937" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D937" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E937" s="12" t="s">
+        <v>1261</v>
+      </c>
+      <c r="F937" s="12" t="s">
+        <v>1345</v>
+      </c>
+      <c r="G937" s="12" t="s">
+        <v>1321</v>
+      </c>
+      <c r="H937" s="12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I937" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J937" s="12" t="s">
+        <v>1117</v>
+      </c>
+      <c r="K937" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="L937" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="M937" s="12" t="s">
+        <v>1122</v>
+      </c>
+      <c r="N937" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A938" s="4"/>

</xml_diff>